<commit_message>
Enda en oppdatering til burndownchart
</commit_message>
<xml_diff>
--- a/BurndownChart/BurndownChart Sprint 1.xlsx
+++ b/BurndownChart/BurndownChart Sprint 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maggi\OneDrive - NTNU\V2019\gruppe-35\BurndownChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{232CA7CB-D6E0-43BC-B4EA-1194387B4FDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{5F535411-B688-454A-9EEF-95FC00814934}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{232CA7CB-D6E0-43BC-B4EA-1194387B4FDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BBA3FEE8-5016-4601-8DB2-D4932BB5F488}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BacklogTable" sheetId="1" r:id="rId1"/>
@@ -967,7 +967,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1121,7 +1121,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2814,7 +2814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -2971,10 +2971,10 @@
         <v>8.5333333333333332</v>
       </c>
       <c r="E9" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>